<commit_message>
exogenous agent params example
</commit_message>
<xml_diff>
--- a/data/input/SimulatorScenarios.xlsx
+++ b/data/input/SimulatorScenarios.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE133C5-DAF5-854B-A410-80EE28E21D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,23 +357,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="235" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -418,7 +419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -429,16 +430,16 @@
         <v>100</v>
       </c>
       <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>10</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exogenous agent params example (#2)
</commit_message>
<xml_diff>
--- a/data/input/SimulatorScenarios.xlsx
+++ b/data/input/SimulatorScenarios.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE133C5-DAF5-854B-A410-80EE28E21D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,23 +357,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="235" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -418,7 +419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -429,16 +430,16 @@
         <v>100</v>
       </c>
       <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>10</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>